<commit_message>
Changes to scripts and folders
</commit_message>
<xml_diff>
--- a/AK/AK_completed_output.xlsx
+++ b/AK/AK_completed_output.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -473,7 +473,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -503,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -533,7 +533,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -563,7 +563,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -623,7 +623,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -683,7 +683,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -743,7 +743,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -863,7 +863,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -893,7 +893,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -923,7 +923,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -983,7 +983,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1013,7 +1013,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1043,7 +1043,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1103,7 +1103,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1163,7 +1163,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1223,7 +1223,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1253,7 +1253,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1283,7 +1283,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1433,7 +1433,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1463,7 +1463,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1643,7 +1643,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1703,7 +1703,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1733,7 +1733,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1763,7 +1763,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1793,7 +1793,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1883,7 +1883,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1913,7 +1913,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -1943,7 +1943,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -1973,7 +1973,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2003,7 +2003,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2033,7 +2033,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2063,7 +2063,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2123,7 +2123,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2153,7 +2153,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
@@ -2273,7 +2273,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2303,7 +2303,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2363,7 +2363,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2423,7 +2423,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2453,7 +2453,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2483,7 +2483,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
@@ -2513,7 +2513,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2543,7 +2543,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2603,7 +2603,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
@@ -2633,7 +2633,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2663,7 +2663,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2693,7 +2693,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -2843,7 +2843,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
@@ -2873,7 +2873,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -2933,7 +2933,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -2963,7 +2963,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
@@ -2993,7 +2993,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3023,7 +3023,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3053,7 +3053,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3083,7 +3083,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3203,7 +3203,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3233,7 +3233,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3263,7 +3263,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3293,7 +3293,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3323,7 +3323,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3353,7 +3353,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3383,7 +3383,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3443,7 +3443,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -3473,7 +3473,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3503,7 +3503,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
@@ -3593,7 +3593,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3623,7 +3623,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3653,7 +3653,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3683,7 +3683,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3743,7 +3743,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -3803,7 +3803,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3833,7 +3833,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -3863,7 +3863,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3893,7 +3893,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -3923,7 +3923,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3953,7 +3953,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -3983,7 +3983,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4043,7 +4043,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4103,7 +4103,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -4193,7 +4193,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4253,7 +4253,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4283,7 +4283,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4343,7 +4343,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4373,7 +4373,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4403,7 +4403,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4433,7 +4433,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4463,7 +4463,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4493,7 +4493,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4523,7 +4523,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4583,7 +4583,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -4613,7 +4613,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4643,7 +4643,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4673,7 +4673,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4703,7 +4703,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4763,7 +4763,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4793,7 +4793,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4823,7 +4823,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4883,7 +4883,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4943,7 +4943,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4973,7 +4973,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -5003,7 +5003,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -5033,7 +5033,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5063,7 +5063,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5123,7 +5123,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5183,7 +5183,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5213,7 +5213,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5243,7 +5243,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -5273,7 +5273,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5303,7 +5303,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5333,7 +5333,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5363,7 +5363,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5423,7 +5423,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5483,7 +5483,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -5513,7 +5513,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -5543,7 +5543,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5573,7 +5573,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -5603,7 +5603,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5633,7 +5633,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -5663,7 +5663,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5693,7 +5693,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -5723,7 +5723,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5753,7 +5753,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -5783,7 +5783,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5813,7 +5813,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -5843,7 +5843,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -5873,7 +5873,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -5903,7 +5903,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5933,7 +5933,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -5963,7 +5963,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
@@ -5993,7 +5993,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -6023,7 +6023,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -6053,7 +6053,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -6083,7 +6083,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -6113,7 +6113,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -6143,7 +6143,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -6173,7 +6173,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -6203,7 +6203,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -6263,7 +6263,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -6323,7 +6323,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -6353,7 +6353,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -6383,7 +6383,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6413,7 +6413,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -6443,7 +6443,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -6473,7 +6473,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -6503,7 +6503,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -6533,7 +6533,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -6563,7 +6563,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -6623,7 +6623,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -6653,7 +6653,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -6683,7 +6683,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -6713,7 +6713,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -6743,7 +6743,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -6773,7 +6773,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -6803,7 +6803,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -6893,7 +6893,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -6923,7 +6923,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -6953,7 +6953,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -6983,7 +6983,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -7013,7 +7013,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -7043,7 +7043,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
@@ -7073,7 +7073,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -7103,7 +7103,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -7163,7 +7163,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
@@ -7193,7 +7193,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -7223,7 +7223,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -7253,7 +7253,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -7283,7 +7283,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
@@ -7313,7 +7313,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -7343,7 +7343,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -7373,7 +7373,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -7403,7 +7403,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
@@ -7433,7 +7433,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -7463,7 +7463,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -7493,7 +7493,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
@@ -7553,7 +7553,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -7583,7 +7583,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -7613,7 +7613,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -7643,7 +7643,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
@@ -7673,7 +7673,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -7703,7 +7703,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -7733,7 +7733,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -7763,7 +7763,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
@@ -7793,7 +7793,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -7823,7 +7823,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -7853,7 +7853,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -7883,7 +7883,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
@@ -7913,7 +7913,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -7943,7 +7943,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -7973,7 +7973,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -8063,7 +8063,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -8093,7 +8093,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -8123,7 +8123,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C257" t="inlineStr">
@@ -8153,7 +8153,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C258" t="inlineStr">
@@ -8183,7 +8183,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C259" t="inlineStr">
@@ -8213,7 +8213,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C260" t="inlineStr">
@@ -8243,7 +8243,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C261" t="inlineStr">
@@ -8273,7 +8273,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C262" t="inlineStr">
@@ -8303,7 +8303,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C263" t="inlineStr">
@@ -8333,7 +8333,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C264" t="inlineStr">
@@ -8363,7 +8363,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C265" t="inlineStr">
@@ -8393,7 +8393,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C266" t="inlineStr">
@@ -8423,7 +8423,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C267" t="inlineStr">
@@ -8453,7 +8453,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C268" t="inlineStr">
@@ -8483,7 +8483,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C269" t="inlineStr">
@@ -8513,7 +8513,7 @@
       </c>
       <c r="B270" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C270" t="inlineStr">
@@ -8543,7 +8543,7 @@
       </c>
       <c r="B271" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C271" t="inlineStr">
@@ -8573,7 +8573,7 @@
       </c>
       <c r="B272" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C272" t="inlineStr">
@@ -8603,7 +8603,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C273" t="inlineStr">
@@ -8633,7 +8633,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C274" t="inlineStr">
@@ -8663,7 +8663,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C275" t="inlineStr">
@@ -8693,7 +8693,7 @@
       </c>
       <c r="B276" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C276" t="inlineStr">
@@ -8723,7 +8723,7 @@
       </c>
       <c r="B277" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C277" t="inlineStr">
@@ -8753,7 +8753,7 @@
       </c>
       <c r="B278" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C278" t="inlineStr">
@@ -8783,7 +8783,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C279" t="inlineStr">
@@ -8813,7 +8813,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C280" t="inlineStr">
@@ -8843,7 +8843,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C281" t="inlineStr">
@@ -8873,7 +8873,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C282" t="inlineStr">
@@ -8903,7 +8903,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C283" t="inlineStr">
@@ -8933,7 +8933,7 @@
       </c>
       <c r="B284" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C284" t="inlineStr">
@@ -8963,7 +8963,7 @@
       </c>
       <c r="B285" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C285" t="inlineStr">
@@ -8993,7 +8993,7 @@
       </c>
       <c r="B286" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C286" t="inlineStr">
@@ -9023,7 +9023,7 @@
       </c>
       <c r="B287" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C287" t="inlineStr">
@@ -9053,7 +9053,7 @@
       </c>
       <c r="B288" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C288" t="inlineStr">
@@ -9083,7 +9083,7 @@
       </c>
       <c r="B289" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C289" t="inlineStr">
@@ -9113,7 +9113,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C290" t="inlineStr">
@@ -9143,7 +9143,7 @@
       </c>
       <c r="B291" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C291" t="inlineStr">
@@ -9173,7 +9173,7 @@
       </c>
       <c r="B292" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C292" t="inlineStr">
@@ -9203,7 +9203,7 @@
       </c>
       <c r="B293" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C293" t="inlineStr">
@@ -9233,7 +9233,7 @@
       </c>
       <c r="B294" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C294" t="inlineStr">
@@ -9263,7 +9263,7 @@
       </c>
       <c r="B295" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C295" t="inlineStr">
@@ -9293,7 +9293,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C296" t="inlineStr">
@@ -9323,7 +9323,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C297" t="inlineStr">
@@ -9353,7 +9353,7 @@
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C298" t="inlineStr">
@@ -9383,7 +9383,7 @@
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C299" t="inlineStr">
@@ -9413,7 +9413,7 @@
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C300" t="inlineStr">
@@ -9443,7 +9443,7 @@
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C301" t="inlineStr">
@@ -9473,7 +9473,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C302" t="inlineStr">
@@ -9503,7 +9503,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C303" t="inlineStr">
@@ -9533,7 +9533,7 @@
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C304" t="inlineStr">
@@ -9563,7 +9563,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C305" t="inlineStr">
@@ -9593,7 +9593,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C306" t="inlineStr">
@@ -9623,7 +9623,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C307" t="inlineStr">
@@ -9653,7 +9653,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C308" t="inlineStr">
@@ -9683,7 +9683,7 @@
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C309" t="inlineStr">
@@ -9713,7 +9713,7 @@
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C310" t="inlineStr">
@@ -9743,7 +9743,7 @@
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C311" t="inlineStr">
@@ -9773,7 +9773,7 @@
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C312" t="inlineStr">
@@ -9803,7 +9803,7 @@
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C313" t="inlineStr">
@@ -9833,7 +9833,7 @@
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C314" t="inlineStr">
@@ -9863,7 +9863,7 @@
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C315" t="inlineStr">
@@ -9893,7 +9893,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C316" t="inlineStr">
@@ -9923,7 +9923,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
@@ -9953,7 +9953,7 @@
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
@@ -9983,7 +9983,7 @@
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C319" t="inlineStr">
@@ -10013,7 +10013,7 @@
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C320" t="inlineStr">
@@ -10043,7 +10043,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>03012025</t>
+          <t>99999999</t>
         </is>
       </c>
       <c r="C321" t="inlineStr">

</xml_diff>